<commit_message>
added: pandas, navigation structure
</commit_message>
<xml_diff>
--- a/testing/Workbook1.xlsx
+++ b/testing/Workbook1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -413,8 +413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="98" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" zoomScalePageLayoutView="98" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -587,6 +587,54 @@
       <c r="E3" s="1">
         <v>42043</v>
       </c>
+      <c r="F3" s="1">
+        <v>42044</v>
+      </c>
+      <c r="G3" s="1">
+        <v>42045</v>
+      </c>
+      <c r="H3" s="1">
+        <v>42046</v>
+      </c>
+      <c r="I3" s="1">
+        <v>42047</v>
+      </c>
+      <c r="J3" s="1">
+        <v>42048</v>
+      </c>
+      <c r="K3" s="1">
+        <v>42049</v>
+      </c>
+      <c r="L3" s="1">
+        <v>42050</v>
+      </c>
+      <c r="M3" s="1">
+        <v>42051</v>
+      </c>
+      <c r="N3" s="1">
+        <v>42052</v>
+      </c>
+      <c r="O3" s="1">
+        <v>42053</v>
+      </c>
+      <c r="P3" s="1">
+        <v>42054</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>42055</v>
+      </c>
+      <c r="R3" s="1">
+        <v>42056</v>
+      </c>
+      <c r="S3" s="1">
+        <v>42057</v>
+      </c>
+      <c r="T3" s="1">
+        <v>42058</v>
+      </c>
+      <c r="U3" s="1">
+        <v>42059</v>
+      </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -603,6 +651,54 @@
       </c>
       <c r="E4" s="1">
         <v>42044</v>
+      </c>
+      <c r="F4" s="1">
+        <v>42045</v>
+      </c>
+      <c r="G4" s="1">
+        <v>42046</v>
+      </c>
+      <c r="H4" s="1">
+        <v>42047</v>
+      </c>
+      <c r="I4" s="1">
+        <v>42048</v>
+      </c>
+      <c r="J4" s="1">
+        <v>42049</v>
+      </c>
+      <c r="K4" s="1">
+        <v>42050</v>
+      </c>
+      <c r="L4" s="1">
+        <v>42051</v>
+      </c>
+      <c r="M4" s="1">
+        <v>42052</v>
+      </c>
+      <c r="N4" s="1">
+        <v>42053</v>
+      </c>
+      <c r="O4" s="1">
+        <v>42054</v>
+      </c>
+      <c r="P4" s="1">
+        <v>42055</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>42056</v>
+      </c>
+      <c r="R4" s="1">
+        <v>42057</v>
+      </c>
+      <c r="S4" s="1">
+        <v>42058</v>
+      </c>
+      <c r="T4" s="1">
+        <v>42059</v>
+      </c>
+      <c r="U4" s="1">
+        <v>42060</v>
       </c>
     </row>
   </sheetData>

</xml_diff>